<commit_message>
Paper Draft V2 related changes
</commit_message>
<xml_diff>
--- a/Figure Generating/MAG_variable_importance.xlsx
+++ b/Figure Generating/MAG_variable_importance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin Juntao\Desktop\transposase-deep-ocean\Figure Generating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292F0ED7-F362-44B3-95B5-EC220C71EAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058ECCAE-55D7-4209-8075-E99CE470407E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
   <si>
     <t>Variable SumSquare (in order)</t>
   </si>
@@ -146,13 +146,101 @@
   </si>
   <si>
     <t>Taxonomy of MAGs (Class)</t>
+  </si>
+  <si>
+    <t>R-square</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>depth + taxon</t>
+  </si>
+  <si>
+    <t>depth + biofilm</t>
+  </si>
+  <si>
+    <t>Explanantory Variable(s)</t>
+  </si>
+  <si>
+    <t>P for F-test</t>
+  </si>
+  <si>
+    <r>
+      <t>2.2 x 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-16</t>
+    </r>
+  </si>
+  <si>
+    <t>depth + gsize (genome size)</t>
+  </si>
+  <si>
+    <t>depth * taxon (+ interaction term)</t>
+  </si>
+  <si>
+    <t>depth * taxon + biofilm + gsize</t>
+  </si>
+  <si>
+    <r>
+      <t>2.2 x 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.7 x 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-6</t>
+    </r>
+  </si>
+  <si>
+    <t>depth * taxon + biofilm + gsize + gsize2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +251,34 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -373,9 +489,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -389,6 +505,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -396,51 +572,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -449,22 +592,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -758,7 +887,7 @@
   <dimension ref="B2:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,7 +895,8 @@
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="23" customWidth="1"/>
     <col min="9" max="9" width="19.77734375" customWidth="1"/>
     <col min="11" max="11" width="4.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.109375" bestFit="1" customWidth="1"/>
@@ -777,7 +907,7 @@
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="22" t="s">
         <v>8</v>
       </c>
     </row>
@@ -788,7 +918,7 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="22">
         <v>0.35070000000000001</v>
       </c>
     </row>
@@ -799,7 +929,7 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="22">
         <v>0.35070000000000001</v>
       </c>
     </row>
@@ -810,7 +940,7 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="22">
         <v>0.35070000000000001</v>
       </c>
     </row>
@@ -832,407 +962,498 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="I16" s="5" t="s">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+    </row>
+    <row r="15" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="15" x14ac:dyDescent="0.3">
+      <c r="D16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="I16" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="J16" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K16" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="L16" s="8"/>
-      <c r="M16" s="9"/>
-    </row>
-    <row r="17" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I17" s="6"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="21" t="s">
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
+    </row>
+    <row r="17" spans="4:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="I17" s="26"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L17" s="17" t="s">
+      <c r="L17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M17" s="22" t="s">
+      <c r="M17" s="15" t="s">
         <v>11</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I18" s="29" t="s">
+    <row r="18" spans="4:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.435</v>
+      </c>
+      <c r="I18" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="30">
-        <f>M18/N18</f>
+      <c r="J18" s="21">
+        <f t="shared" ref="J18:J34" si="0">M18/N18</f>
         <v>0.90909090909090906</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="5">
         <v>1</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="6">
         <v>0</v>
       </c>
-      <c r="M18" s="12">
+      <c r="M18" s="7">
         <v>10</v>
       </c>
       <c r="N18">
-        <f>SUM(K18:M18)</f>
+        <f t="shared" ref="N18:N34" si="1">SUM(K18:M18)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I19" s="25" t="s">
+    <row r="19" spans="4:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="D19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="I19" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="19">
-        <f>M19/N19</f>
+      <c r="J19" s="12">
+        <f t="shared" si="0"/>
         <v>0.81818181818181823</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="5">
         <v>2</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="6">
         <v>0</v>
       </c>
-      <c r="M19" s="12">
+      <c r="M19" s="7">
         <v>9</v>
       </c>
       <c r="N19">
-        <f>SUM(K19:M19)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I20" s="29" t="s">
+    <row r="20" spans="4:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="D20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="I20" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="30">
-        <f>M20/N20</f>
+      <c r="J20" s="21">
+        <f t="shared" si="0"/>
         <v>0.56981132075471697</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="5">
         <v>63</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="6">
         <v>51</v>
       </c>
-      <c r="M20" s="12">
+      <c r="M20" s="7">
         <v>151</v>
       </c>
       <c r="N20">
-        <f>SUM(K20:M20)</f>
+        <f t="shared" si="1"/>
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I21" s="25" t="s">
+    <row r="21" spans="4:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="D21" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="I21" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="19">
-        <f>M21/N21</f>
+      <c r="J21" s="12">
+        <f t="shared" si="0"/>
         <v>0.52631578947368418</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="5">
         <v>0</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L21" s="6">
         <v>9</v>
       </c>
-      <c r="M21" s="12">
+      <c r="M21" s="7">
         <v>10</v>
       </c>
       <c r="N21">
-        <f>SUM(K21:M21)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I22" s="29" t="s">
+    <row r="22" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="22">
+        <v>1.1E-4</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="I22" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J22" s="30">
-        <f>M22/N22</f>
+      <c r="J22" s="21">
+        <f t="shared" si="0"/>
         <v>0.46488294314381273</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="5">
         <v>89</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="6">
         <v>71</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M22" s="7">
         <v>139</v>
       </c>
       <c r="N22">
-        <f>SUM(K22:M22)</f>
+        <f t="shared" si="1"/>
         <v>299</v>
       </c>
     </row>
-    <row r="23" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I23" s="29" t="s">
+    <row r="23" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="I23" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="30">
-        <f>M23/N23</f>
+      <c r="J23" s="21">
+        <f t="shared" si="0"/>
         <v>0.45833333333333331</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="5">
         <v>6</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="6">
         <v>7</v>
       </c>
-      <c r="M23" s="12">
+      <c r="M23" s="7">
         <v>11</v>
       </c>
       <c r="N23">
-        <f>SUM(K23:M23)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I24" s="29" t="s">
+    <row r="24" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="I24" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J24" s="30">
-        <f>M24/N24</f>
+      <c r="J24" s="21">
+        <f t="shared" si="0"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="5">
         <v>15</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="6">
         <v>5</v>
       </c>
-      <c r="M24" s="12">
+      <c r="M24" s="7">
         <v>15</v>
       </c>
       <c r="N24">
-        <f>SUM(K24:M24)</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I25" s="29" t="s">
+    <row r="25" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D25" s="22"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="22"/>
+      <c r="I25" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="J25" s="30">
-        <f>M25/N25</f>
+      <c r="J25" s="21">
+        <f t="shared" si="0"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="5">
         <v>2</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="6">
         <v>6</v>
       </c>
-      <c r="M25" s="12">
+      <c r="M25" s="7">
         <v>6</v>
       </c>
       <c r="N25">
-        <f>SUM(K25:M25)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I26" s="25" t="s">
+    <row r="26" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="I26" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="19">
-        <f>M26/N26</f>
+      <c r="J26" s="12">
+        <f t="shared" si="0"/>
         <v>0.38709677419354838</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26" s="5">
         <v>5</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L26" s="6">
         <v>14</v>
       </c>
-      <c r="M26" s="12">
+      <c r="M26" s="7">
         <v>12</v>
       </c>
       <c r="N26">
-        <f>SUM(K26:M26)</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I27" s="25" t="s">
+    <row r="27" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="I27" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="J27" s="19">
-        <f>M27/N27</f>
+      <c r="J27" s="12">
+        <f t="shared" si="0"/>
         <v>0.34375</v>
       </c>
-      <c r="K27" s="10">
+      <c r="K27" s="5">
         <v>5</v>
       </c>
-      <c r="L27" s="11">
+      <c r="L27" s="6">
         <v>16</v>
       </c>
-      <c r="M27" s="12">
+      <c r="M27" s="7">
         <v>11</v>
       </c>
       <c r="N27">
-        <f>SUM(K27:M27)</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I28" s="25" t="s">
+    <row r="28" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="I28" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="19">
-        <f>M28/N28</f>
+      <c r="J28" s="12">
+        <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="5">
         <v>2</v>
       </c>
-      <c r="L28" s="11">
+      <c r="L28" s="6">
         <v>15</v>
       </c>
-      <c r="M28" s="12">
+      <c r="M28" s="7">
         <v>8</v>
       </c>
       <c r="N28">
-        <f>SUM(K28:M28)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I29" s="25" t="s">
+    <row r="29" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="I29" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J29" s="19">
-        <f>M29/N29</f>
+      <c r="J29" s="12">
+        <f t="shared" si="0"/>
         <v>0.2862595419847328</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="5">
         <v>83</v>
       </c>
-      <c r="L29" s="11">
+      <c r="L29" s="6">
         <v>104</v>
       </c>
-      <c r="M29" s="12">
+      <c r="M29" s="7">
         <v>75</v>
       </c>
       <c r="N29">
-        <f>SUM(K29:M29)</f>
+        <f t="shared" si="1"/>
         <v>262</v>
       </c>
     </row>
-    <row r="30" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I30" s="25" t="s">
+    <row r="30" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="I30" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="J30" s="19">
-        <f>M30/N30</f>
+      <c r="J30" s="12">
+        <f t="shared" si="0"/>
         <v>0.28387096774193549</v>
       </c>
-      <c r="K30" s="10">
+      <c r="K30" s="5">
         <v>78</v>
       </c>
-      <c r="L30" s="11">
+      <c r="L30" s="6">
         <v>33</v>
       </c>
-      <c r="M30" s="12">
+      <c r="M30" s="7">
         <v>44</v>
       </c>
       <c r="N30">
-        <f>SUM(K30:M30)</f>
+        <f t="shared" si="1"/>
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I31" s="27" t="s">
+    <row r="31" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="I31" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="J31" s="28">
-        <f>M31/N31</f>
+      <c r="J31" s="19">
+        <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K31" s="5">
         <v>12</v>
       </c>
-      <c r="L31" s="11">
+      <c r="L31" s="6">
         <v>24</v>
       </c>
-      <c r="M31" s="12">
+      <c r="M31" s="7">
         <v>14</v>
       </c>
       <c r="N31">
-        <f>SUM(K31:M31)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I32" s="25" t="s">
+    <row r="32" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="I32" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J32" s="19">
-        <f>M32/N32</f>
+      <c r="J32" s="12">
+        <f t="shared" si="0"/>
         <v>0.19047619047619047</v>
       </c>
-      <c r="K32" s="10">
+      <c r="K32" s="5">
         <v>6</v>
       </c>
-      <c r="L32" s="11">
+      <c r="L32" s="6">
         <v>11</v>
       </c>
-      <c r="M32" s="12">
+      <c r="M32" s="7">
         <v>4</v>
       </c>
       <c r="N32">
-        <f>SUM(K32:M32)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
     <row r="33" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I33" s="27" t="s">
+      <c r="I33" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="J33" s="28">
-        <f>M33/N33</f>
+      <c r="J33" s="19">
+        <f t="shared" si="0"/>
         <v>8.1081081081081086E-2</v>
       </c>
-      <c r="K33" s="10">
+      <c r="K33" s="5">
         <v>15</v>
       </c>
-      <c r="L33" s="11">
+      <c r="L33" s="6">
         <v>19</v>
       </c>
-      <c r="M33" s="12">
+      <c r="M33" s="7">
         <v>3</v>
       </c>
       <c r="N33">
-        <f>SUM(K33:M33)</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
     </row>
     <row r="34" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I34" s="26" t="s">
+      <c r="I34" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="J34" s="20">
-        <f>M34/N34</f>
+      <c r="J34" s="13">
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="K34" s="13">
+      <c r="K34" s="8">
         <v>10</v>
       </c>
-      <c r="L34" s="14">
+      <c r="L34" s="9">
         <v>5</v>
       </c>
-      <c r="M34" s="15">
+      <c r="M34" s="10">
         <v>1</v>
       </c>
       <c r="N34">
-        <f>SUM(K34:M34)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
@@ -1246,11 +1467,11 @@
         <v>394</v>
       </c>
       <c r="L35" s="1">
-        <f t="shared" ref="L35:M35" si="0">SUM(L18:L34)</f>
+        <f>SUM(L18:L34)</f>
         <v>390</v>
       </c>
       <c r="M35" s="1">
-        <f t="shared" si="0"/>
+        <f>SUM(M18:M34)</f>
         <v>523</v>
       </c>
       <c r="N35">
@@ -1264,6 +1485,7 @@
     <mergeCell ref="J16:J17"/>
     <mergeCell ref="K16:M16"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1319,17 +1541,17 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="9"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="31"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1346,15 +1568,15 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="21" t="s">
+      <c r="H3" s="33"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="15" t="s">
         <v>11</v>
       </c>
       <c r="M3" s="1" t="s">
@@ -1376,24 +1598,24 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="30">
-        <f>L4/M4</f>
+      <c r="I4" s="21">
+        <f t="shared" ref="I4:I20" si="0">L4/M4</f>
         <v>0.90909090909090906</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="5">
         <v>1</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="6">
         <v>0</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="7">
         <v>10</v>
       </c>
       <c r="M4">
-        <f>SUM(J4:L4)</f>
+        <f t="shared" ref="M4:M20" si="1">SUM(J4:L4)</f>
         <v>11</v>
       </c>
     </row>
@@ -1412,24 +1634,24 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="19">
-        <f>L5/M5</f>
+      <c r="I5" s="12">
+        <f t="shared" si="0"/>
         <v>0.81818181818181823</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="5">
         <v>2</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="6">
         <v>0</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="7">
         <v>9</v>
       </c>
       <c r="M5">
-        <f>SUM(J5:L5)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
@@ -1448,24 +1670,24 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="30">
-        <f>L6/M6</f>
+      <c r="I6" s="21">
+        <f t="shared" si="0"/>
         <v>0.56981132075471697</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="5">
         <v>63</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="6">
         <v>51</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="7">
         <v>151</v>
       </c>
       <c r="M6">
-        <f>SUM(J6:L6)</f>
+        <f t="shared" si="1"/>
         <v>265</v>
       </c>
     </row>
@@ -1484,24 +1706,24 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="19">
-        <f>L7/M7</f>
+      <c r="I7" s="12">
+        <f t="shared" si="0"/>
         <v>0.52631578947368418</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="5">
         <v>0</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="6">
         <v>9</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="7">
         <v>10</v>
       </c>
       <c r="M7">
-        <f>SUM(J7:L7)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -1520,24 +1742,24 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="30">
-        <f>L8/M8</f>
+      <c r="I8" s="21">
+        <f t="shared" si="0"/>
         <v>0.46488294314381273</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="5">
         <v>89</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="6">
         <v>71</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="7">
         <v>139</v>
       </c>
       <c r="M8">
-        <f>SUM(J8:L8)</f>
+        <f t="shared" si="1"/>
         <v>299</v>
       </c>
     </row>
@@ -1556,24 +1778,24 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="30">
-        <f>L9/M9</f>
+      <c r="I9" s="21">
+        <f t="shared" si="0"/>
         <v>0.45833333333333331</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="5">
         <v>6</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="6">
         <v>7</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="7">
         <v>11</v>
       </c>
       <c r="M9">
-        <f>SUM(J9:L9)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
@@ -1592,24 +1814,24 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="30">
-        <f>L10/M10</f>
+      <c r="I10" s="21">
+        <f t="shared" si="0"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="5">
         <v>15</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="6">
         <v>5</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="7">
         <v>15</v>
       </c>
       <c r="M10">
-        <f>SUM(J10:L10)</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
     </row>
@@ -1628,24 +1850,24 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="30">
-        <f>L11/M11</f>
+      <c r="I11" s="21">
+        <f t="shared" si="0"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="5">
         <v>2</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="6">
         <v>6</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="7">
         <v>6</v>
       </c>
       <c r="M11">
-        <f>SUM(J11:L11)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
@@ -1664,24 +1886,24 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="19">
-        <f>L12/M12</f>
+      <c r="I12" s="12">
+        <f t="shared" si="0"/>
         <v>0.38709677419354838</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="5">
         <v>5</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="6">
         <v>14</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="7">
         <v>12</v>
       </c>
       <c r="M12">
-        <f>SUM(J12:L12)</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
     </row>
@@ -1700,24 +1922,24 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="19">
-        <f>L13/M13</f>
+      <c r="I13" s="12">
+        <f t="shared" si="0"/>
         <v>0.34375</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="5">
         <v>5</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="6">
         <v>16</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="7">
         <v>11</v>
       </c>
       <c r="M13">
-        <f>SUM(J13:L13)</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
     </row>
@@ -1736,24 +1958,24 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="19">
-        <f>L14/M14</f>
+      <c r="I14" s="12">
+        <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="5">
         <v>2</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="6">
         <v>15</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="7">
         <v>8</v>
       </c>
       <c r="M14">
-        <f>SUM(J14:L14)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
@@ -1772,24 +1994,24 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="19">
-        <f>L15/M15</f>
+      <c r="I15" s="12">
+        <f t="shared" si="0"/>
         <v>0.2862595419847328</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="5">
         <v>83</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="6">
         <v>104</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="7">
         <v>75</v>
       </c>
       <c r="M15">
-        <f>SUM(J15:L15)</f>
+        <f t="shared" si="1"/>
         <v>262</v>
       </c>
     </row>
@@ -1808,24 +2030,24 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="19">
-        <f>L16/M16</f>
+      <c r="I16" s="12">
+        <f t="shared" si="0"/>
         <v>0.28387096774193549</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="5">
         <v>78</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="6">
         <v>33</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="7">
         <v>44</v>
       </c>
       <c r="M16">
-        <f>SUM(J16:L16)</f>
+        <f t="shared" si="1"/>
         <v>155</v>
       </c>
     </row>
@@ -1844,24 +2066,24 @@
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="H17" s="27" t="s">
+      <c r="H17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="28">
-        <f>L17/M17</f>
+      <c r="I17" s="19">
+        <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="5">
         <v>12</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="6">
         <v>24</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="7">
         <v>14</v>
       </c>
       <c r="M17">
-        <f>SUM(J17:L17)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
@@ -1880,24 +2102,24 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="19">
-        <f>L18/M18</f>
+      <c r="I18" s="12">
+        <f t="shared" si="0"/>
         <v>0.19047619047619047</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="5">
         <v>6</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="6">
         <v>11</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L18" s="7">
         <v>4</v>
       </c>
       <c r="M18">
-        <f>SUM(J18:L18)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
@@ -1907,53 +2129,53 @@
         <v>25.90117647058824</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:D19" si="0">SUM(C2:C18)/17</f>
+        <f>SUM(C2:C18)/17</f>
         <v>33.871176470588239</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f>SUM(D2:D18)/17</f>
         <v>40.22941176470588</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="28">
-        <f>L19/M19</f>
+      <c r="I19" s="19">
+        <f t="shared" si="0"/>
         <v>8.1081081081081086E-2</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="5">
         <v>15</v>
       </c>
-      <c r="K19" s="11">
+      <c r="K19" s="6">
         <v>19</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="7">
         <v>3</v>
       </c>
       <c r="M19">
-        <f>SUM(J19:L19)</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H20" s="26" t="s">
+      <c r="H20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="20">
-        <f>L20/M20</f>
+      <c r="I20" s="13">
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="8">
         <v>10</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="9">
         <v>5</v>
       </c>
-      <c r="L20" s="15">
+      <c r="L20" s="10">
         <v>1</v>
       </c>
       <c r="M20">
-        <f>SUM(J20:L20)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
@@ -1967,11 +2189,11 @@
         <v>394</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" ref="K21:L21" si="1">SUM(K4:K20)</f>
+        <f>SUM(K4:K20)</f>
         <v>390</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="1"/>
+        <f>SUM(L4:L20)</f>
         <v>523</v>
       </c>
       <c r="M21">

</xml_diff>